<commit_message>
📝 MAJ du JDT
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_ThodeMateo.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_ThodeMateo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Modules\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F1EE93-67A5-4DF2-952D-F7108CFA56F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A583ECDD-56DD-4219-93B9-FD382EFB6033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -70,12 +70,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{0E6A8FB1-09AF-453E-8B87-CF7157F791DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mateo Gabriel Thode:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+3h</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -201,6 +225,18 @@
   </si>
   <si>
     <t>Document ci-présent</t>
+  </si>
+  <si>
+    <t>Gestion des erreurs 400</t>
+  </si>
+  <si>
+    <t>Gestion des erreurs 500 avec Axios</t>
+  </si>
+  <si>
+    <t>Fonctionne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne fonctionne pas encore. </t>
   </si>
 </sst>
 </file>
@@ -540,80 +576,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -781,6 +743,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1144,16 +1180,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15277777777777779</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6388888888888895E-2</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8611111111111112E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1868,18 +1904,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2073,9 +2109,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2128,7 +2164,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 5 minutes</v>
+        <v>0 jours 16 heurs 45 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2143,15 +2179,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>600</v>
+        <v>660</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>245</v>
+        <v>345</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>845</v>
+        <v>1005</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2508,58 +2544,98 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45798</v>
+      </c>
       <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+      <c r="D18" s="48">
+        <v>10</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45798</v>
+      </c>
       <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="56"/>
+      <c r="D19" s="52">
+        <v>45</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>44</v>
+      </c>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="55"/>
+        <v>21</v>
+      </c>
+      <c r="B20" s="46">
+        <v>45798</v>
+      </c>
+      <c r="C20" s="47">
+        <v>1</v>
+      </c>
+      <c r="D20" s="48">
+        <v>35</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
+      <c r="A21" s="16">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="50">
+        <v>45798</v>
+      </c>
       <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="56"/>
+      <c r="D21" s="52">
+        <v>10</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
@@ -8700,28 +8776,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8796,11 +8872,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8808,7 +8884,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.15277777777777779</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8836,7 +8912,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8844,7 +8920,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>7.6388888888888895E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8854,7 +8930,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8862,7 +8938,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>4.8611111111111112E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8925,7 +9001,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.58680555555555558</v>
+        <v>0.69791666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8948,6 +9024,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9170,17 +9257,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9190,6 +9266,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9206,15 +9293,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>